<commit_message>
Creación de tokens, inicio y cierre de sesión con token y mejora en modelo user
</commit_message>
<xml_diff>
--- a/Reportes/proyectos.xlsx
+++ b/Reportes/proyectos.xlsx
@@ -9,9 +9,7 @@
   <sheets>
     <sheet name="Listado Proyectos" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Listado Proyectos'!$C$3:$F$4</definedName>
-  </definedNames>
+  <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
@@ -28,8 +26,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <name val="Times"/>
       <b val="1"/>
+      <color rgb="00FFFFFF"/>
       <sz val="12"/>
     </font>
   </fonts>
@@ -41,10 +39,7 @@
       <patternFill patternType="gray125"/>
     </fill>
     <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00ADD8E6"/>
-        <bgColor rgb="00ADD8E6"/>
-      </patternFill>
+      <patternFill patternType="solid"/>
     </fill>
   </fills>
   <borders count="2">
@@ -155,7 +150,7 @@
     <tableColumn id="5" name="Inversión"/>
     <tableColumn id="6" name="Fecha Inicio"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="1"/>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -456,7 +451,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="23" customWidth="1" min="3" max="3"/>
+    <col width="22" customWidth="1" min="3" max="3"/>
     <col width="25" customWidth="1" min="4" max="4"/>
     <col width="14" customWidth="1" min="5" max="5"/>
     <col width="17" customWidth="1" min="6" max="6"/>
@@ -489,25 +484,24 @@
     <row r="4">
       <c r="C4" t="inlineStr">
         <is>
-          <t>Proyecto de prueba</t>
+          <t>Proyecto prueba 2</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Proyecto de prueba 1</t>
+          <t>añsdfkjañsldasñdlfkj</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>1500000</v>
+        <v>2000000000</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>15/01/2025</t>
+          <t>21/01/2025</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="C3:F4"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <tableParts count="1">
     <tablePart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>

</xml_diff>